<commit_message>
TEMPLATES CORRETOS E GERA??O TAMB?M
</commit_message>
<xml_diff>
--- a/services/templates/padrao_Total_Contas.xlsx
+++ b/services/templates/padrao_Total_Contas.xlsx
@@ -44,13 +44,13 @@
     <t>SALDO</t>
   </si>
   <si>
-    <t>CONTROLE DE PROJETOS - SALDO DOS PROJETOS</t>
-  </si>
-  <si>
     <t>CONTA</t>
   </si>
   <si>
     <t>PROJETO(S)</t>
+  </si>
+  <si>
+    <t>CONTROLE DE PROJETOS -TOTAL DAS CONTAS</t>
   </si>
 </sst>
 </file>
@@ -172,13 +172,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +464,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -499,10 +499,10 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="11"/>
@@ -535,16 +535,16 @@
       <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="10" t="s">
         <v>5</v>
       </c>

</xml_diff>